<commit_message>
new local charges saving and calculating - waiting on new offer calculator
Former-commit-id: cbb105d9ba49050056d97f03b4c234ecf1cec307
</commit_message>
<xml_diff>
--- a/db/dummydata/st_freight_rates.xlsx
+++ b/db/dummydata/st_freight_rates.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="43">
   <si>
     <t>CUSTOMER_ID</t>
   </si>
@@ -104,6 +104,42 @@
   </si>
   <si>
     <t>Taichung</t>
+  </si>
+  <si>
+    <t>Dubai</t>
+  </si>
+  <si>
+    <t>Jeddah</t>
+  </si>
+  <si>
+    <t>Melbourne</t>
+  </si>
+  <si>
+    <t>cheapest</t>
+  </si>
+  <si>
+    <t>fast</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>Shanghai</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>Beijing</t>
+  </si>
+  <si>
+    <t>fastest</t>
+  </si>
+  <si>
+    <t>Xiamen</t>
+  </si>
+  <si>
+    <t>Tianjin</t>
   </si>
 </sst>
 </file>
@@ -113,7 +149,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -127,6 +163,15 @@
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -136,13 +181,18 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -169,6 +219,24 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -403,6 +471,713 @@
         <v>60.0</v>
       </c>
     </row>
+    <row r="5">
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="5">
+        <v>43177.0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>43547.0</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="6">
+        <v>20.0</v>
+      </c>
+      <c r="K5" s="8">
+        <v>1000.0</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P5" s="10">
+        <v>8.0</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="5">
+        <v>43178.0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>43548.0</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="6">
+        <v>20.0</v>
+      </c>
+      <c r="K6" s="8">
+        <v>1000.0</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="12">
+        <v>33.0</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>33.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="5">
+        <v>43179.0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>43549.0</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="6">
+        <v>44.0</v>
+      </c>
+      <c r="K7" s="8">
+        <v>1000.0</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" s="6">
+        <v>15.0</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="5">
+        <v>43180.0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>43550.0</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="6">
+        <v>39.0</v>
+      </c>
+      <c r="K8" s="8">
+        <v>1000.0</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P8" s="6">
+        <v>19.0</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="D9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="5">
+        <v>43181.0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>43551.0</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" s="6">
+        <v>44.0</v>
+      </c>
+      <c r="K9" s="8">
+        <v>1000.0</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" s="6">
+        <v>15.0</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="D10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="5">
+        <v>43182.0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>43552.0</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="6">
+        <v>41.0</v>
+      </c>
+      <c r="K10" s="8">
+        <v>1000.0</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10" s="6">
+        <v>23.0</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>23.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="D11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="5">
+        <v>43183.0</v>
+      </c>
+      <c r="G11" s="5">
+        <v>43553.0</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" s="6">
+        <v>30.0</v>
+      </c>
+      <c r="K11" s="8">
+        <v>1000.0</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P11" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="D12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="5">
+        <v>43184.0</v>
+      </c>
+      <c r="G12" s="5">
+        <v>43554.0</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="6">
+        <v>32.0</v>
+      </c>
+      <c r="K12" s="8">
+        <v>1000.0</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="6">
+        <v>8.0</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="D13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="5">
+        <v>43185.0</v>
+      </c>
+      <c r="G13" s="5">
+        <v>43555.0</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="6">
+        <v>48.0</v>
+      </c>
+      <c r="K13" s="8">
+        <v>1000.0</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P13" s="6">
+        <v>45.0</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>45.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="D14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="5">
+        <v>43186.0</v>
+      </c>
+      <c r="G14" s="5">
+        <v>43556.0</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J14" s="6">
+        <v>35.0</v>
+      </c>
+      <c r="K14" s="8">
+        <v>1000.0</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P14" s="6">
+        <v>67.0</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>67.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="D15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="5">
+        <v>43187.0</v>
+      </c>
+      <c r="G15" s="5">
+        <v>43557.0</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J15" s="6">
+        <v>41.0</v>
+      </c>
+      <c r="K15" s="8">
+        <v>1000.0</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P15" s="6">
+        <v>28.0</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>28.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="D16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="5">
+        <v>43188.0</v>
+      </c>
+      <c r="G16" s="5">
+        <v>43558.0</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" s="6">
+        <v>33.0</v>
+      </c>
+      <c r="K16" s="8">
+        <v>1000.0</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P16" s="6">
+        <v>58.0</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>58.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="D17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="5">
+        <v>43189.0</v>
+      </c>
+      <c r="G17" s="5">
+        <v>43559.0</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="6">
+        <v>36.0</v>
+      </c>
+      <c r="K17" s="8">
+        <v>1000.0</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P17" s="6">
+        <v>50.0</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="D18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="5">
+        <v>43190.0</v>
+      </c>
+      <c r="G18" s="5">
+        <v>43560.0</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" s="6">
+        <v>40.0</v>
+      </c>
+      <c r="K18" s="8">
+        <v>1000.0</v>
+      </c>
+      <c r="L18" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P18" s="6">
+        <v>10.0</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="D19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="5">
+        <v>43191.0</v>
+      </c>
+      <c r="G19" s="5">
+        <v>43561.0</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J19" s="6">
+        <v>33.0</v>
+      </c>
+      <c r="K19" s="8">
+        <v>1000.0</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P19" s="6">
+        <v>27.0</v>
+      </c>
+      <c r="Q19" s="6">
+        <v>27.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="D20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="5">
+        <v>43192.0</v>
+      </c>
+      <c r="G20" s="5">
+        <v>43562.0</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" s="6">
+        <v>38.0</v>
+      </c>
+      <c r="K20" s="8">
+        <v>1000.0</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P20" s="6">
+        <v>14.0</v>
+      </c>
+      <c r="Q20" s="6">
+        <v>14.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="K21" s="8"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>